<commit_message>
I am seeing how to handle recursive lambdas
</commit_message>
<xml_diff>
--- a/Excel_Challenge_526 - Next 3 Palindromes.xlsx
+++ b/Excel_Challenge_526 - Next 3 Palindromes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6D7D05-972D-4207-8C00-58E3E7715C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD4D70F-B657-4B09-90DE-2F1BB97F7F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="EDA" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>Number</t>
   </si>
@@ -780,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F10E52-4419-4819-B746-BA54FD1D9675}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,4 +1060,177 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8662DEAC-0F6B-404A-8580-96B00388DB50}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>121</v>
+      </c>
+      <c r="D2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>367</v>
+      </c>
+      <c r="B3">
+        <v>373</v>
+      </c>
+      <c r="C3">
+        <v>383</v>
+      </c>
+      <c r="D3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>818</v>
+      </c>
+      <c r="B4">
+        <v>828</v>
+      </c>
+      <c r="C4">
+        <v>838</v>
+      </c>
+      <c r="D4">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3045</v>
+      </c>
+      <c r="B5">
+        <v>3113</v>
+      </c>
+      <c r="C5">
+        <v>3223</v>
+      </c>
+      <c r="D5">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>13672</v>
+      </c>
+      <c r="B6">
+        <v>13731</v>
+      </c>
+      <c r="C6">
+        <v>13831</v>
+      </c>
+      <c r="D6">
+        <v>13931</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>237847</v>
+      </c>
+      <c r="B7">
+        <v>238832</v>
+      </c>
+      <c r="C7">
+        <v>239932</v>
+      </c>
+      <c r="D7">
+        <v>240042</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8304747</v>
+      </c>
+      <c r="B8">
+        <v>8305038</v>
+      </c>
+      <c r="C8">
+        <v>8306038</v>
+      </c>
+      <c r="D8">
+        <v>8307038</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>39965382</v>
+      </c>
+      <c r="B9">
+        <v>39966993</v>
+      </c>
+      <c r="C9">
+        <v>39977993</v>
+      </c>
+      <c r="D9">
+        <v>39988993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>734203527</v>
+      </c>
+      <c r="B10">
+        <v>734212437</v>
+      </c>
+      <c r="C10">
+        <v>734222437</v>
+      </c>
+      <c r="D10">
+        <v>734232437</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" cm="1">
+        <f t="array" ref="B15">_xlfn.LET(_xlpm.x,100,
+     _xlpm.r, _xlfn.LAMBDA(_xlpm.r,_xlpm.n,
+                  IF(
+                     _xlpm.n = --_xlfn.CONCAT(MID(_xlpm.n, 10 - ROW(1:9), 1)),
+                     _xlpm.n,
+                     _xlpm.r(_xlpm.r, 1 + _xlpm.n)
+                    )
+               ),
+     _xlpm.r(_xlpm.r,_xlpm.x+1)
+)</f>
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
My EDA contains a single function
</commit_message>
<xml_diff>
--- a/Excel_Challenge_526 - Next 3 Palindromes.xlsx
+++ b/Excel_Challenge_526 - Next 3 Palindromes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD4D70F-B657-4B09-90DE-2F1BB97F7F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA2396A-1611-4A46-A917-6C859482FCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,6 +609,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1064,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8662DEAC-0F6B-404A-8580-96B00388DB50}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,18 +1218,201 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" cm="1">
-        <f t="array" ref="B15">_xlfn.LET(_xlpm.x,100,
-     _xlpm.r, _xlfn.LAMBDA(_xlpm.r,_xlpm.n,
-                  IF(
-                     _xlpm.n = --_xlfn.CONCAT(MID(_xlpm.n, 10 - ROW(1:9), 1)),
-                     _xlpm.n,
-                     _xlpm.r(_xlpm.r, 1 + _xlpm.n)
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15:D23">_xlfn.LET(
+      _xlpm.r, _xlfn.LAMBDA(_xlpm.r,_xlpm.n,
+         IF(
+            _xlpm.n = --_xlfn.CONCAT(MID(_xlpm.n, 10 - ROW(1:9), 1)),
+            _xlpm.n,
+            _xlpm.r(_xlpm.r, 1 + _xlpm.n)
+          )
+          ),
+      _xlpm.z, _xlfn.MAP(A2:A10,
+          _xlfn.LAMBDA(_xlpm.x,
+                 _xlfn.LET(_xlpm.i,{1,2,3},
+                     _xlfn.TEXTJOIN(",",,_xlfn.SCAN(_xlpm.x,_xlpm.i,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.r(_xlpm.r,_xlpm.a+1))))
                     )
-               ),
-     _xlpm.r(_xlpm.r,_xlpm.x+1)
+                )
+           ),
+      _xlfn.DROP(_xlfn.REDUCE(0,_xlpm.z,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,",")))),1)
 )</f>
-        <v>101</v>
+        <v>111</v>
+      </c>
+      <c r="C15" t="str">
+        <v>121</v>
+      </c>
+      <c r="D15" t="str">
+        <v>131</v>
+      </c>
+      <c r="F15" t="b" cm="1">
+        <f t="array" ref="F15:H23">_xlfn.ANCHORARRAY(B15)+0=B2:D10</f>
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <v>373</v>
+      </c>
+      <c r="C16" t="str">
+        <v>383</v>
+      </c>
+      <c r="D16" t="str">
+        <v>393</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <v>828</v>
+      </c>
+      <c r="C17" t="str">
+        <v>838</v>
+      </c>
+      <c r="D17" t="str">
+        <v>848</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <v>3113</v>
+      </c>
+      <c r="C18" t="str">
+        <v>3223</v>
+      </c>
+      <c r="D18" t="str">
+        <v>3333</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <v>13731</v>
+      </c>
+      <c r="C19" t="str">
+        <v>13831</v>
+      </c>
+      <c r="D19" t="str">
+        <v>13931</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <v>238832</v>
+      </c>
+      <c r="C20" t="str">
+        <v>239932</v>
+      </c>
+      <c r="D20" t="str">
+        <v>240042</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <v>8305038</v>
+      </c>
+      <c r="C21" t="str">
+        <v>8306038</v>
+      </c>
+      <c r="D21" t="str">
+        <v>8307038</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <v>39966993</v>
+      </c>
+      <c r="C22" t="str">
+        <v>39977993</v>
+      </c>
+      <c r="D22" t="str">
+        <v>39988993</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <v>734212437</v>
+      </c>
+      <c r="C23" t="str">
+        <v>734222437</v>
+      </c>
+      <c r="D23" t="str">
+        <v>734232437</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>